<commit_message>
Updated with demo user and password for db use cases
</commit_message>
<xml_diff>
--- a/db/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/db/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\december-release\microservices-lowcode-testautomation\db\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\december-release\microservices-lowcode-testautomation\db\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB222A-6553-4EDE-83F2-5D88FB71512F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D3689B-9AA6-4536-AB1C-EA700AB4322A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId1"/>
@@ -110,7 +110,7 @@
     <t>AddifyVariables</t>
   </si>
   <si>
-    <t>quoteId=32633</t>
+    <t>quoteId=184</t>
   </si>
 </sst>
 </file>
@@ -935,31 +935,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.83984375" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="4" max="4" width="27.83984375" customWidth="1"/>
+    <col min="5" max="5" width="20.26171875" customWidth="1"/>
+    <col min="6" max="6" width="70.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83984375" customWidth="1"/>
+    <col min="8" max="8" width="16.15625" customWidth="1"/>
+    <col min="9" max="9" width="14.83984375" customWidth="1"/>
+    <col min="10" max="10" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.578125" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="88.85546875" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="88.83984375" customWidth="1"/>
+    <col min="15" max="15" width="24.578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Updated with Idaithalam DB testing
</commit_message>
<xml_diff>
--- a/db/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/db/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\december-release\microservices-lowcode-testautomation\db\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\jan-release\microservices-lowcode-testautomation\db\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D3689B-9AA6-4536-AB1C-EA700AB4322A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A936C2D-873C-494A-A74E-696794569594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="CSS-Accept-DB" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>quoteId=184</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>Read record</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDB Verify</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDB Select</t>
   </si>
 </sst>
 </file>
@@ -289,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -306,6 +318,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -614,8 +628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:N2" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:N2" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:N3" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:N3" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{2529773C-869E-4BF0-BA40-3C63A1B9C82E}" name="TestCaseName" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{38B39313-4971-4AB8-90FF-17FEEBD272E2}" name="Type" dataDxfId="12"/>
@@ -933,33 +947,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83984375" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="27.83984375" customWidth="1"/>
-    <col min="5" max="5" width="20.26171875" customWidth="1"/>
-    <col min="6" max="6" width="70.41796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83984375" customWidth="1"/>
-    <col min="8" max="8" width="16.15625" customWidth="1"/>
-    <col min="9" max="9" width="14.83984375" customWidth="1"/>
-    <col min="10" max="10" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.578125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="88.83984375" customWidth="1"/>
-    <col min="15" max="15" width="24.578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="88.85546875" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1020,10 +1034,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" t="s">
@@ -1035,15 +1049,44 @@
       <c r="K2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="12"/>
       <c r="P2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with additional information for multipart form
</commit_message>
<xml_diff>
--- a/db/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/db/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\jan-release\microservices-lowcode-testautomation\db\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A936C2D-873C-494A-A74E-696794569594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8958CF6B-70AF-4D5A-B496-8CF4752BB465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -90,39 +90,39 @@
     <t>InsuranceQuoteByDB</t>
   </si>
   <si>
-    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [quoteId]
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>EvaluateFunctionVariables</t>
+  </si>
+  <si>
+    <t>AddifyVariables</t>
+  </si>
+  <si>
+    <t>VERIFY</t>
+  </si>
+  <si>
+    <t>Read record</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDB Verify</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDB Select</t>
+  </si>
+  <si>
+    <t>request_Id=184</t>
+  </si>
+  <si>
+    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [request_Id]</t>
+  </si>
+  <si>
+    <t>policy_limit_amount=[0].policy_limit_amount;quoteId=[0].id;</t>
+  </si>
+  <si>
+    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [request_Id]
 id,insurance_premium_amount, insurance_premium_currency, policy_limit_amount
-i~[quoteId],d~500.00,CHF,d~50000.00</t>
-  </si>
-  <si>
-    <t>policy_limit_amount=[0].policy_limit_amount</t>
-  </si>
-  <si>
-    <t>SELECT</t>
-  </si>
-  <si>
-    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [quoteId]</t>
-  </si>
-  <si>
-    <t>EvaluateFunctionVariables</t>
-  </si>
-  <si>
-    <t>AddifyVariables</t>
-  </si>
-  <si>
-    <t>quoteId=184</t>
-  </si>
-  <si>
-    <t>VERIFY</t>
-  </si>
-  <si>
-    <t>Read record</t>
-  </si>
-  <si>
-    <t>InsuranceQuoteByDB Verify</t>
-  </si>
-  <si>
-    <t>InsuranceQuoteByDB Select</t>
+[quoteId],d~500.00,CHF,d~50000.00</t>
   </si>
 </sst>
 </file>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
     <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="54.5703125" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="88.85546875" customWidth="1"/>
     <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -1017,10 +1017,10 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -1034,29 +1034,29 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="12"/>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -1070,14 +1070,14 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1086,7 +1086,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="4"/>
       <c r="N3" s="8" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with new release version 1.5.0
</commit_message>
<xml_diff>
--- a/db/src/test/resources/css/customer-self-service-with-db.xlsx
+++ b/db/src/test/resources/css/customer-self-service-with-db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\jan-release\microservices-lowcode-testautomation\db\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8958CF6B-70AF-4D5A-B496-8CF4752BB465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C771F22-B6C7-44F6-B64B-5CEA2D3BB968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -84,45 +84,35 @@
     <t>StepInfo</t>
   </si>
   <si>
-    <t>verify record</t>
-  </si>
-  <si>
     <t>InsuranceQuoteByDB</t>
   </si>
   <si>
+    <t>EvaluateFunctionVariables</t>
+  </si>
+  <si>
+    <t>AddifyVariables</t>
+  </si>
+  <si>
+    <t>InsuranceQuoteByDB Select</t>
+  </si>
+  <si>
+    <t>request_Id=184</t>
+  </si>
+  <si>
+    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [request_Id]</t>
+  </si>
+  <si>
+    <t>policy_limit_amount=[0].policy_limit_amount;quoteId=[0].id;</t>
+  </si>
+  <si>
     <t>SELECT</t>
   </si>
   <si>
-    <t>EvaluateFunctionVariables</t>
-  </si>
-  <si>
-    <t>AddifyVariables</t>
-  </si>
-  <si>
-    <t>VERIFY</t>
-  </si>
-  <si>
-    <t>Read record</t>
-  </si>
-  <si>
-    <t>InsuranceQuoteByDB Verify</t>
-  </si>
-  <si>
-    <t>InsuranceQuoteByDB Select</t>
-  </si>
-  <si>
-    <t>request_Id=184</t>
-  </si>
-  <si>
-    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [request_Id]</t>
-  </si>
-  <si>
-    <t>policy_limit_amount=[0].policy_limit_amount;quoteId=[0].id;</t>
-  </si>
-  <si>
-    <t>select iqr.id, iq.insurance_premium_amount, iq.insurance_premium_currency, iq.policy_limit_amount from insurancequotes iq INNER JOIN insurancequoterequests iqr on iq.id = iqr.insurance_quote_id and iqr.id  =  [request_Id]
-id,insurance_premium_amount, insurance_premium_currency, policy_limit_amount
-[quoteId],d~500.00,CHF,d~50000.00</t>
+    <t>id,insurance_premium_amount, insurance_premium_currency, policy_limit_amount
+i~[request_Id],d~500.00,CHF,d~50000.00</t>
+  </si>
+  <si>
+    <t>get insurance quote id;for insurance premium;query;information on the;insurance premium;</t>
   </si>
 </sst>
 </file>
@@ -308,11 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -320,6 +306,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,6 +467,7 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -628,8 +621,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:N3" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:N3" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:N2" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:N2" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{2529773C-869E-4BF0-BA40-3C63A1B9C82E}" name="TestCaseName" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{38B39313-4971-4AB8-90FF-17FEEBD272E2}" name="Type" dataDxfId="12"/>
@@ -947,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +952,7 @@
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
@@ -974,13 +967,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -995,13 +988,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1013,19 +1006,19 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -1034,59 +1027,31 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="13"/>
+      <c r="K2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="11"/>
       <c r="M2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="10"/>
       <c r="P2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>